<commit_message>
add - generate inner rule info
</commit_message>
<xml_diff>
--- a/kaiyuanyouce/task003/day5_openpyxl/openpyxl_demo.xlsx
+++ b/kaiyuanyouce/task003/day5_openpyxl/openpyxl_demo.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="默认创建的工作簿" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,23 +14,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
-  <si>
-    <t>Pentest</t>
-  </si>
-  <si>
-    <t>公众号: FullStackPentest</t>
-  </si>
-  <si>
-    <t>大数据测试</t>
-  </si>
-  <si>
-    <t>Python3</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,15 +46,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -372,48 +423,72 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>测试开发</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>测试开发</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>测试开发</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>测试开发</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>测试开发</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>测试开发</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>公众号: FullStackPentest</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>公众号: FullStackPentest</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>公众号: FullStackPentest</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>公众号: FullStackPentest</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>公众号: FullStackPentest</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>公众号: FullStackPentest</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -431,48 +506,72 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>测试开发1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>测试开发1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>测试开发1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>测试开发1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>测试开发1</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>测试开发1</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>大数据测试</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>大数据测试</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>大数据测试</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>大数据测试</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>大数据测试</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>大数据测试</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -490,47 +589,71 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>测试开发2</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>测试开发2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>测试开发2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>测试开发2</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>测试开发2</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>测试开发2</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update - fix conflict
</commit_message>
<xml_diff>
--- a/kaiyuanyouce/task003/day5_openpyxl/openpyxl_demo.xlsx
+++ b/kaiyuanyouce/task003/day5_openpyxl/openpyxl_demo.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="默认创建的工作簿" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,6 +14,23 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+  <si>
+    <t>Pentest</t>
+  </si>
+  <si>
+    <t>公众号: FullStackPentest</t>
+  </si>
+  <si>
+    <t>大数据测试</t>
+  </si>
+  <si>
+    <t>Python3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,83 +63,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -423,72 +372,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>测试开发</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>测试开发</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>测试开发</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>测试开发</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>测试开发</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>测试开发</t>
-        </is>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>公众号: FullStackPentest</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>公众号: FullStackPentest</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>公众号: FullStackPentest</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>公众号: FullStackPentest</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>公众号: FullStackPentest</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>公众号: FullStackPentest</t>
-        </is>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -506,72 +431,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>测试开发1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>测试开发1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>测试开发1</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>测试开发1</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>测试开发1</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>测试开发1</t>
-        </is>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>大数据测试</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>大数据测试</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>大数据测试</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>大数据测试</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>大数据测试</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>大数据测试</t>
-        </is>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -589,71 +490,47 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>测试开发2</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>测试开发2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>测试开发2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>测试开发2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>测试开发2</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>测试开发2</t>
-        </is>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Python3</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Python3</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Python3</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Python3</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Python3</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Python3</t>
-        </is>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>